<commit_message>
fix get_classe_LnLs - lq[root_nodenum] for a change in updated diversitree
</commit_message>
<xml_diff>
--- a/ex/cinthy/Labels_speciesTrees.xlsx
+++ b/ex/cinthy/Labels_speciesTrees.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjim882/Dropbox/Epacrid_project/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmat471/HD/GitHub/PhyBEARS.jl/ex/cinthy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7E9A92-1618-CA48-B98F-5CA0AAC4E831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ACB484-8526-5142-BF3E-58EB6400DBD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{EEE896E7-D973-AE4D-BEA7-BF160C9EB19C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="50320" windowHeight="28300" xr2:uid="{EEE896E7-D973-AE4D-BEA7-BF160C9EB19C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,10 +29,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2101,7 +2101,7 @@
   <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3355,10 +3355,10 @@
         <v>19</v>
       </c>
       <c r="J33" t="s">
-        <v>456</v>
+        <v>9</v>
       </c>
       <c r="K33" t="s">
-        <v>9</v>
+        <v>456</v>
       </c>
       <c r="L33" t="s">
         <v>456</v>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/nmatzke/PhyBEARS.jl"
This reverts commit 261cf0ff8b4b9cec9354f9f1924066c2885d0788, reversing
changes made to 3f06d2dd85c971100dfaf305d3377799e9b1fbf2.
</commit_message>
<xml_diff>
--- a/ex/cinthy/Labels_speciesTrees.xlsx
+++ b/ex/cinthy/Labels_speciesTrees.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmat471/HD/GitHub/PhyBEARS.jl/ex/cinthy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjim882/Dropbox/Epacrid_project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ACB484-8526-5142-BF3E-58EB6400DBD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7E9A92-1618-CA48-B98F-5CA0AAC4E831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="50320" windowHeight="28300" xr2:uid="{EEE896E7-D973-AE4D-BEA7-BF160C9EB19C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{EEE896E7-D973-AE4D-BEA7-BF160C9EB19C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,10 +29,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2101,7 +2101,7 @@
   <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3355,10 +3355,10 @@
         <v>19</v>
       </c>
       <c r="J33" t="s">
+        <v>456</v>
+      </c>
+      <c r="K33" t="s">
         <v>9</v>
-      </c>
-      <c r="K33" t="s">
-        <v>456</v>
       </c>
       <c r="L33" t="s">
         <v>456</v>

</xml_diff>